<commit_message>
Have imperfect forumla versions of updating time and comparison visuals - chugging along making updates for ALFS ppt. Have not pushed website updates in a few days
</commit_message>
<xml_diff>
--- a/data/ucues_2022_rebuild.xlsx
+++ b/data/ucues_2022_rebuild.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sanolan\OneDrive\IR_Folder\UCSD_Gaps_Quarto\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E858DDF9-774D-4B4E-A80F-A763BA09A173}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6566FAB-9F43-4637-AD98-A123A9E72F9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -758,7 +758,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -769,8 +769,8 @@
   <dimension ref="A1:N1865"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A204" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H337" sqref="H337"/>
+      <pane ySplit="1" topLeftCell="A535" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J554" sqref="J554"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -18452,6 +18452,12 @@
       <c r="H553">
         <v>3</v>
       </c>
+      <c r="I553" s="6">
+        <v>0</v>
+      </c>
+      <c r="J553">
+        <v>0</v>
+      </c>
     </row>
     <row r="554" spans="1:10">
       <c r="A554" t="s">

</xml_diff>

<commit_message>
adding more visuals to acex added acex questions to gses data file
</commit_message>
<xml_diff>
--- a/data/ucues_2022_rebuild.xlsx
+++ b/data/ucues_2022_rebuild.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sanolan\OneDrive\IR_Folder\UCSD_Gaps_Quarto\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA96E791-5358-4CC1-9D91-CBB4CE4B06E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F2BCB4B-06B7-48C6-BA2D-77A1595FDEDA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -772,8 +772,8 @@
   <dimension ref="A1:N1865"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A659" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A674" sqref="A674"/>
+      <pane ySplit="1" topLeftCell="A243" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A182" sqref="A182"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>

</xml_diff>